<commit_message>
Got my single function
</commit_message>
<xml_diff>
--- a/CH-133 Custom Grouping.xlsx
+++ b/CH-133 Custom Grouping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510AAE40-E3FA-4CA2-A695-58B485DD87CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1EB8AC6-4671-4CF9-ADC3-AB4F8CB74DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -776,6 +776,88 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>709246</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>158263</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>398584</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>128955</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Callout: Double Bent Line 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F26F7F58-FBEF-3F05-EA7F-0D56BEE9609F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3341077" y="5246078"/>
+          <a:ext cx="1635369" cy="334108"/>
+        </a:xfrm>
+        <a:prstGeom prst="borderCallout3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 18750"/>
+            <a:gd name="adj2" fmla="val -8333"/>
+            <a:gd name="adj3" fmla="val 18750"/>
+            <a:gd name="adj4" fmla="val -16667"/>
+            <a:gd name="adj5" fmla="val 100000"/>
+            <a:gd name="adj6" fmla="val -16667"/>
+            <a:gd name="adj7" fmla="val 188887"/>
+            <a:gd name="adj8" fmla="val -108333"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>Improperly</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t> grouped</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Basis">
   <a:themeElements>
@@ -1604,8 +1686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDAF7AD6-8F80-47D0-944A-CA90F6591593}">
   <dimension ref="A1:N88"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C48" sqref="B43:C48"/>
+    <sheetView topLeftCell="A79" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2477,8 +2559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90E96D0F-80BF-4F83-9610-3AD58A04C663}">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3019,6 +3101,16 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
+      <c r="K22" s="5" cm="1">
+        <f t="array" ref="K22:L27">_xlfn.LET(
+_xlpm.d, _xlfn.MAP(B3:B40,_xlfn.LAMBDA(_xlpm.x,_xlfn.LET(_xlpm.y,DAY(_xlpm.x),(MEDIAN(1,_xlpm.y,10)=_xlpm.y)*1+(MEDIAN(11,20,_xlpm.y)=_xlpm.y)*2+(MEDIAN(21,31,_xlpm.y)=_xlpm.y)*3+(MONTH(_xlpm.x)-1)*3 ))),
+_xlfn.GROUPBY(_xlpm.d,C3:C40,_xleta.SUM,,0)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>117</v>
+      </c>
       <c r="N22" s="2"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
@@ -3037,6 +3129,12 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
+      <c r="K23" s="4">
+        <v>2</v>
+      </c>
+      <c r="L23">
+        <v>339</v>
+      </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B24" s="15">
@@ -3053,6 +3151,12 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
+      <c r="K24" s="4">
+        <v>3</v>
+      </c>
+      <c r="L24">
+        <v>110</v>
+      </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B25" s="15">
@@ -3069,6 +3173,12 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
+      <c r="K25" s="4">
+        <v>4</v>
+      </c>
+      <c r="L25">
+        <v>254</v>
+      </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B26" s="15">
@@ -3085,6 +3195,12 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
+      <c r="K26" s="4">
+        <v>5</v>
+      </c>
+      <c r="L26">
+        <v>512</v>
+      </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B27" s="15">
@@ -3100,6 +3216,12 @@
       <c r="E27" s="36">
         <f t="shared" si="1"/>
         <v>5</v>
+      </c>
+      <c r="K27" s="4">
+        <v>6</v>
+      </c>
+      <c r="L27">
+        <v>297</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
@@ -3318,5 +3440,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added commentary on today's work
</commit_message>
<xml_diff>
--- a/CH-133 Custom Grouping.xlsx
+++ b/CH-133 Custom Grouping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1D65B7-B092-4C55-89A6-C3F754488B69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A02350-B4B2-4A6F-80F2-54291B4806EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="18">
   <si>
     <t>Question</t>
   </si>
@@ -113,6 +113,12 @@
   </si>
   <si>
     <t>Data to Add</t>
+  </si>
+  <si>
+    <t>I am making a simple note because I just spent 3 hours working on a battery spreadsheet.</t>
+  </si>
+  <si>
+    <t>I am taking this time as Excel practice time for today.</t>
   </si>
 </sst>
 </file>
@@ -410,6 +416,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -420,11 +431,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1150,19 +1156,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="32"/>
+      <c r="C1" s="35"/>
       <c r="E1"/>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="34"/>
-      <c r="K1" s="33" t="s">
+      <c r="H1" s="37"/>
+      <c r="K1" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="34"/>
+      <c r="L1" s="37"/>
       <c r="N1" s="7" t="s">
         <v>13</v>
       </c>
@@ -1708,19 +1714,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="32"/>
+      <c r="C1" s="35"/>
       <c r="E1"/>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="34"/>
-      <c r="K1" s="33" t="s">
+      <c r="H1" s="37"/>
+      <c r="K1" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="34"/>
+      <c r="L1" s="37"/>
       <c r="N1" s="7" t="s">
         <v>13</v>
       </c>
@@ -2565,8 +2571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90E96D0F-80BF-4F83-9610-3AD58A04C663}">
   <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G17" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2582,19 +2588,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="32"/>
+      <c r="C1" s="35"/>
       <c r="E1"/>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="34"/>
-      <c r="K1" s="33" t="s">
+      <c r="H1" s="37"/>
+      <c r="K1" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="34"/>
+      <c r="L1" s="37"/>
       <c r="N1" s="7" t="s">
         <v>13</v>
       </c>
@@ -2628,11 +2634,11 @@
       <c r="C3" s="16">
         <v>39</v>
       </c>
-      <c r="D3" s="35">
+      <c r="D3" s="31">
         <f>DAY(B3)</f>
         <v>5</v>
       </c>
-      <c r="E3" s="36">
+      <c r="E3" s="32">
         <f>(MEDIAN(1,D3,10)=D3)*1+(MEDIAN(11,20,D3)=D3)*2+(MEDIAN(21,31,D3)=D3)*3 +(MONTH(B3)-1)*3</f>
         <v>1</v>
       </c>
@@ -2651,6 +2657,9 @@
         <v>117</v>
       </c>
       <c r="M3" s="9"/>
+      <c r="N3" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B4" s="15">
@@ -2659,11 +2668,11 @@
       <c r="C4" s="16">
         <v>78</v>
       </c>
-      <c r="D4" s="35">
+      <c r="D4" s="31">
         <f t="shared" ref="D4:D40" si="0">DAY(B4)</f>
         <v>9</v>
       </c>
-      <c r="E4" s="36">
+      <c r="E4" s="32">
         <f t="shared" ref="E4:E40" si="1">(MEDIAN(1,D4,10)=D4)*1+(MEDIAN(11,20,D4)=D4)*2+(MEDIAN(21,31,D4)=D4)*3 +(MONTH(B4)-1)*3</f>
         <v>1</v>
       </c>
@@ -2682,6 +2691,9 @@
         <v>339</v>
       </c>
       <c r="M4" s="9"/>
+      <c r="N4" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="17">
@@ -2690,11 +2702,11 @@
       <c r="C5" s="18">
         <v>7</v>
       </c>
-      <c r="D5" s="35">
+      <c r="D5" s="31">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="E5" s="36">
+      <c r="E5" s="32">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -2721,11 +2733,11 @@
       <c r="C6" s="18">
         <v>84</v>
       </c>
-      <c r="D6" s="35">
+      <c r="D6" s="31">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="32">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -2752,11 +2764,11 @@
       <c r="C7" s="18">
         <v>81</v>
       </c>
-      <c r="D7" s="35">
+      <c r="D7" s="31">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="32">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -2781,11 +2793,11 @@
       <c r="C8" s="18">
         <v>24</v>
       </c>
-      <c r="D8" s="35">
+      <c r="D8" s="31">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="32">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -2813,11 +2825,11 @@
       <c r="C9" s="18">
         <v>32</v>
       </c>
-      <c r="D9" s="35">
+      <c r="D9" s="31">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E9" s="32">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -2837,11 +2849,11 @@
       <c r="C10" s="18">
         <v>56</v>
       </c>
-      <c r="D10" s="35">
+      <c r="D10" s="31">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="E10" s="36">
+      <c r="E10" s="32">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -2861,11 +2873,11 @@
       <c r="C11" s="18">
         <v>38</v>
       </c>
-      <c r="D11" s="35">
+      <c r="D11" s="31">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="E11" s="36">
+      <c r="E11" s="32">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -2885,11 +2897,11 @@
       <c r="C12" s="18">
         <v>11</v>
       </c>
-      <c r="D12" s="35">
+      <c r="D12" s="31">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="E12" s="36">
+      <c r="E12" s="32">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -2910,11 +2922,11 @@
       <c r="C13" s="18">
         <v>3</v>
       </c>
-      <c r="D13" s="35">
+      <c r="D13" s="31">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="E13" s="36">
+      <c r="E13" s="32">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -2933,11 +2945,11 @@
       <c r="C14" s="18">
         <v>3</v>
       </c>
-      <c r="D14" s="35">
+      <c r="D14" s="31">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="E14" s="36">
+      <c r="E14" s="32">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -2956,11 +2968,11 @@
       <c r="C15" s="16">
         <v>4</v>
       </c>
-      <c r="D15" s="35">
+      <c r="D15" s="31">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="E15" s="36">
+      <c r="E15" s="32">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -2979,11 +2991,11 @@
       <c r="C16" s="16">
         <v>59</v>
       </c>
-      <c r="D16" s="35">
+      <c r="D16" s="31">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="E16" s="36">
+      <c r="E16" s="32">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -3002,11 +3014,11 @@
       <c r="C17" s="16">
         <v>30</v>
       </c>
-      <c r="D17" s="35">
+      <c r="D17" s="31">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="E17" s="36">
+      <c r="E17" s="32">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -3025,11 +3037,11 @@
       <c r="C18" s="16">
         <v>17</v>
       </c>
-      <c r="D18" s="35">
+      <c r="D18" s="31">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="E18" s="36">
+      <c r="E18" s="32">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -3048,11 +3060,11 @@
       <c r="C19" s="18">
         <v>79</v>
       </c>
-      <c r="D19" s="35">
+      <c r="D19" s="31">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E19" s="36">
+      <c r="E19" s="32">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
@@ -3065,11 +3077,11 @@
       <c r="C20" s="18">
         <v>79</v>
       </c>
-      <c r="D20" s="35">
+      <c r="D20" s="31">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E20" s="36">
+      <c r="E20" s="32">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
@@ -3082,11 +3094,11 @@
       <c r="C21" s="18">
         <v>29</v>
       </c>
-      <c r="D21" s="35">
+      <c r="D21" s="31">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="E21" s="36">
+      <c r="E21" s="32">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
@@ -3099,11 +3111,11 @@
       <c r="C22" s="18">
         <v>21</v>
       </c>
-      <c r="D22" s="35">
+      <c r="D22" s="31">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="E22" s="36">
+      <c r="E22" s="32">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
@@ -3129,11 +3141,11 @@
       <c r="C23" s="18">
         <v>46</v>
       </c>
-      <c r="D23" s="35">
+      <c r="D23" s="31">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E23" s="36">
+      <c r="E23" s="32">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
@@ -3153,11 +3165,11 @@
       <c r="C24" s="16">
         <v>27</v>
       </c>
-      <c r="D24" s="35">
+      <c r="D24" s="31">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="E24" s="36">
+      <c r="E24" s="32">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -3177,11 +3189,11 @@
       <c r="C25" s="16">
         <v>50</v>
       </c>
-      <c r="D25" s="35">
+      <c r="D25" s="31">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="E25" s="36">
+      <c r="E25" s="32">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -3201,11 +3213,11 @@
       <c r="C26" s="16">
         <v>95</v>
       </c>
-      <c r="D26" s="35">
+      <c r="D26" s="31">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="E26" s="36">
+      <c r="E26" s="32">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -3225,11 +3237,11 @@
       <c r="C27" s="16">
         <v>58</v>
       </c>
-      <c r="D27" s="35">
+      <c r="D27" s="31">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="E27" s="36">
+      <c r="E27" s="32">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -3249,11 +3261,11 @@
       <c r="C28" s="16">
         <v>57</v>
       </c>
-      <c r="D28" s="35">
+      <c r="D28" s="31">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="E28" s="36">
+      <c r="E28" s="32">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -3273,11 +3285,11 @@
       <c r="C29" s="16">
         <v>97</v>
       </c>
-      <c r="D29" s="35">
+      <c r="D29" s="31">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="E29" s="36">
+      <c r="E29" s="32">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -3297,11 +3309,11 @@
       <c r="C30" s="16">
         <v>6</v>
       </c>
-      <c r="D30" s="35">
+      <c r="D30" s="31">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="E30" s="36">
+      <c r="E30" s="32">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -3321,11 +3333,11 @@
       <c r="C31" s="16">
         <v>71</v>
       </c>
-      <c r="D31" s="35">
+      <c r="D31" s="31">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="E31" s="36">
+      <c r="E31" s="32">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -3337,11 +3349,11 @@
       <c r="C32" s="16">
         <v>40</v>
       </c>
-      <c r="D32" s="35">
+      <c r="D32" s="31">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="E32" s="36">
+      <c r="E32" s="32">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -3353,11 +3365,11 @@
       <c r="C33" s="18">
         <v>11</v>
       </c>
-      <c r="D33" s="35">
+      <c r="D33" s="31">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="32">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -3369,11 +3381,11 @@
       <c r="C34" s="18">
         <v>96</v>
       </c>
-      <c r="D34" s="35">
+      <c r="D34" s="31">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="32">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
@@ -3385,11 +3397,11 @@
       <c r="C35" s="18">
         <v>19</v>
       </c>
-      <c r="D35" s="35">
+      <c r="D35" s="31">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="E35" s="36">
+      <c r="E35" s="32">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
@@ -3401,11 +3413,11 @@
       <c r="C36" s="18">
         <v>54</v>
       </c>
-      <c r="D36" s="35">
+      <c r="D36" s="31">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="E36" s="36">
+      <c r="E36" s="32">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
@@ -3417,11 +3429,11 @@
       <c r="C37" s="18">
         <v>17</v>
       </c>
-      <c r="D37" s="35">
+      <c r="D37" s="31">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="E37" s="36">
+      <c r="E37" s="32">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
@@ -3433,11 +3445,11 @@
       <c r="C38" s="18">
         <v>1</v>
       </c>
-      <c r="D38" s="35">
+      <c r="D38" s="31">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="E38" s="36">
+      <c r="E38" s="32">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
@@ -3449,11 +3461,11 @@
       <c r="C39" s="18">
         <v>24</v>
       </c>
-      <c r="D39" s="35">
+      <c r="D39" s="31">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="E39" s="36">
+      <c r="E39" s="32">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
@@ -3465,11 +3477,11 @@
       <c r="C40" s="20">
         <v>86</v>
       </c>
-      <c r="D40" s="35">
+      <c r="D40" s="31">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="E40" s="36">
+      <c r="E40" s="32">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
@@ -3478,7 +3490,7 @@
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B41" s="37">
+      <c r="B41" s="33">
         <v>45352</v>
       </c>
       <c r="C41">
@@ -3486,7 +3498,7 @@
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B42" s="37">
+      <c r="B42" s="33">
         <v>45353</v>
       </c>
       <c r="C42">
@@ -3494,7 +3506,7 @@
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B43" s="37">
+      <c r="B43" s="33">
         <v>45363</v>
       </c>
       <c r="C43">
@@ -3502,7 +3514,7 @@
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="H45" s="37">
+      <c r="H45" s="33">
         <v>45352</v>
       </c>
       <c r="I45">
@@ -3510,7 +3522,7 @@
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="H46" s="37">
+      <c r="H46" s="33">
         <v>45353</v>
       </c>
       <c r="I46">
@@ -3518,7 +3530,7 @@
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="H47" s="37">
+      <c r="H47" s="33">
         <v>45363</v>
       </c>
       <c r="I47">

</xml_diff>